<commit_message>
Added other implementations by ChatGPT
</commit_message>
<xml_diff>
--- a/Experiment Tracking Sheet.xlsx
+++ b/Experiment Tracking Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\natal\Desktop\DIssertation\Ticket5ellingSystem-Exp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44F49C0C-17FA-40E0-BA35-779DAED8FBB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AE995B8-D9F2-4BDB-A2EF-14E7ADBA5004}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23148" yWindow="5880" windowWidth="23256" windowHeight="12456" xr2:uid="{20830222-D529-4FF8-BDA5-3DAE3BD48417}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="58">
   <si>
     <t>Exp #</t>
   </si>
@@ -406,6 +406,576 @@
   </si>
   <si>
     <t>All output are logged</t>
+  </si>
+  <si>
+    <t>Now we will focus on the client program. Based on the outline that you generated for the client program. Please implement steps 1 to 3 in Python to create the base for the client: 1. Initialize the Client Set up initial variables: Initialize a user balance of $4,000 and a local ticket database capable of storing up to 15 tickets. Connect to the server: Use the provided hostname and port to establish a TCP connection with the server. 2. Handle Concurrent Operations Set up threading or multiprocessing: Since the client needs to handle automated requests to the server and listen to another client simultaneously, use a separate thread or process. This allows the client to manage TCP requests/responses with the server while also operating a UDP server to handle incoming SCALP requests. UDP socket setup: Establish a UDP socket on the port number given to the client program +1. This will be used to listen to SCALP requests from the other client. 3. Automated Buy/Sell Requests to Server • Send BUY requests: For each of the 15 transactions, send a BUY request to the server with the current user balance. Depending on the server's response, the client will: o Ticket and price received: Update the local database with the new ticket, adjust the user balance, and continue to the next request. o NOFUNDS: Choose a ticket to sell, send a SELL request to the server, update the user balance with the received funds, and remove the ticket from the local database. o SOLDOUT: Transition to buying tickets from the other client (scalper) using SCALP requests. Please incorporate logging in the program. Make sure to log every output that is printed out on the screen, any errors, any exceptions, any messages received and sent. Save the log in the format of &lt;program_name.log&gt;</t>
+  </si>
+  <si>
+    <t>0/client-0-6.py</t>
+  </si>
+  <si>
+    <t>To implement the client program based on your requirements and incorporate logging for comprehensive tracking of all activities, here’s a detailed Python script. This script sets up the client, handles concurrent operations through threading, manages automated buy/sell requests to the server, and logs all significant events and interactions:
+import socket
+import threading
+import random
+import logging
+import time
+# Configure logging
+logging.basicConfig(level=logging.INFO,
+                    format='%(asctime)s - %(levelname)s - %(message)s',
+                    handlers=[
+                        logging.FileHandler("ticket_client.log"),  # Log file name
+                        logging.StreamHandler()  # Log to stdout
+                    ])
+# Initialize client variables
+user_balance = 4000
+ticket_db = {}  # Local ticket database
+hostname = 'localhost'
+tcp_port = 12345
+udp_port = tcp_port + 1  # UDP port is one more than the TCP port
+def udp_listener():
+    """ Listens for messages on the UDP socket """
+    udp_sock = socket.socket(socket.AF_INET, socket.SOCK_DGRAM)
+    udp_sock.bind((hostname, udp_port))
+    while True:
+        try:
+            data, addr = udp_sock.recvfrom(1024)
+            message = data.decode()
+            logging.info(f"Received SCALP request: {message} from {addr}")
+            # Process SCALP request here (not implemented in this snippet)
+        except Exception as e:
+            logging.error(f"UDP Listener error: {e}")
+            break
+    udp_sock.close()
+def send_requests_to_server(tcp_socket):
+    """ Sends automated BUY requests to the server and handles responses """
+    global user_balance
+    for _ in range(15):  # Simulate 15 transactions
+        try:
+            request = f"BUY {user_balance}"
+            tcp_socket.sendall(request.encode())
+            logging.info(f"Sent to server: {request}")
+            response = tcp_socket.recv(1024).decode()
+            logging.info(f"Received from server: {response}")
+            if response.startswith('NOFUNDS'):
+                # Select a ticket to sell (simplified: select the first one)
+                if ticket_db:
+                    ticket_number, ticket_price = next(iter(ticket_db.items()))
+                    sell_request = f"SELL {ticket_number}"
+                    tcp_socket.sendall(sell_request.encode())
+                    user_balance += ticket_price
+                    del ticket_db[ticket_number]
+                    logging.info(f"Sold ticket {ticket_number} back to server, updated balance: {user_balance}")
+            elif response.startswith('SOLDOUT'):
+                # Process buying tickets from scalper here (not implemented)
+                pass
+            else:
+                ticket_number, price = response.split()
+                ticket_db[ticket_number] = int(price)
+                user_balance -= int(price)
+                logging.info(f"Bought ticket {ticket_number} for ${price}, updated balance: {user_balance}")
+        except Exception as e:
+            logging.error(f"Error during transaction: {e}")
+            break
+    tcp_socket.close()
+def start_client():
+    # Connect to the server
+    tcp_socket = socket.socket(socket.AF_INET, socket.SOCK_STREAM)
+    tcp_socket.connect((hostname, tcp_port))
+    # Set up UDP listener in a separate thread
+    udp_thread = threading.Thread(target=udp_listener)
+    udp_thread.start()
+    # Send requests to the server
+    send_requests_to_server(tcp_socket)
+    udp_thread.join()
+    logging.info("Client operations completed.")
+if __name__ == "__main__":
+    start_client()
+Key Components:
+Logging: All interactions, including sending and receiving messages to/from both TCP and UDP sockets, errors, and significant client state changes, are logged.
+TCP Connection: Handles connection to the server for sending buy/sell requests.
+UDP Server: Runs concurrently in a separate thread to handle incoming SCALP requests from the other client.
+Buy/Sell Logic: Simulates sending buy requests to the server, handles insufficient funds by selling tickets, and attempts to buy from another client when sold out.
+Logging Details:
+Every message sent to and received from the server is logged.
+All errors and exceptions are captured in the log.
+Log output is both printed to the console and saved to ticket_client.log.
+This Python script sets up the client for robust interaction with a server, ensures all important operations are logged, and manages concurrent network operations using threading.</t>
+  </si>
+  <si>
+    <t>Server Log</t>
+  </si>
+  <si>
+    <t>Client Log</t>
+  </si>
+  <si>
+    <t>server-0-3.log</t>
+  </si>
+  <si>
+    <t>server-0-4-na.log</t>
+  </si>
+  <si>
+    <t>server-0-5-client-0-6.log</t>
+  </si>
+  <si>
+    <t>client-0-6-1-server-0-5.log, client-0-6-2-server-0-5.log</t>
+  </si>
+  <si>
+    <t>Attached is the server program that you implemented. However, there are several errors. The first error was that the server did not wait for the second client to connect, but proceeded to sell tickets to the first client. The server is supposed to wait for both clients to connect and then start processing the sell requests from both clients. Please fix this problem given the server program that you implemented.</t>
+  </si>
+  <si>
+    <t>To address the issue where the server begins processing requests before both clients are connected, we need to ensure that all client connections are established before any transaction processing starts. We can do this by coordinating the connections using synchronization mechanisms like threading barriers or condition variables.
+Here's a modified version of the provided server code snippet that implements such a synchronization mechanism to ensure both clients are connected before proceeding with handling their requests:
+import socket
+import threading
+import random
+import logging
+# Configure logging
+logging.basicConfig(level=logging.INFO,
+                    format='%(asctime)s - %(levelname)s - %(message)s',
+                    handlers=[
+                        logging.FileHandler("ticket_server.log"),
+                        logging.StreamHandler()
+                    ])
+# Global lock for thread safety
+lock = threading.Lock()
+# Global ticket database
+tickets = {f"{10000 + i}": {"price": random.randint(200, 400), "sold": False} for i in range(25)}
+# Connection barrier to wait for both clients
+connection_barrier = threading.Barrier(2)  # Set to 2, for two clients
+def handle_client(client_socket, address):
+    global tickets
+    transaction_log = []
+    # Wait for all clients to connect
+    try:
+        connection_barrier.wait()
+    except threading.BrokenBarrierError:
+        logging.error("Barrier is broken due to some client disconnection!")
+        return
+    while True:
+        try:
+            data = client_socket.recv(1024).decode('utf-8').strip()
+            if not data:
+                break
+            logging.info(f"Received from {address}: {data}")
+            cmd, *args = data.split()
+            # Process BUY request
+            if cmd == "BUY":
+                user_balance = int(args[0])
+                response = "SOLDOUT"
+                with lock:
+                    for ticket, details in tickets.items():
+                        if not details['sold'] and user_balance &gt;= details['price']:
+                            if user_balance &gt;= details['price']:
+                                details['sold'] = True
+                                response = f"{ticket} {details['price']}"
+                                transaction_log.append((ticket, 'BUY'))
+                                break
+                            else:
+                                response = "NOFUNDS"
+                                break
+                client_socket.sendall(response.encode())
+            # Process SELL request
+            elif cmd == "SELL":
+                ticket_number = args[0]
+                with lock:
+                    if ticket_number in tickets and tickets[ticket_number]['sold']:
+                        tickets[ticket_number]['sold'] = False
+                        response = f"{ticket_number} {tickets[ticket_number]['price']}"
+                        transaction_log.append((ticket_number, 'SELL'))
+                        client_socket.sendall(response.encode())
+                    else:
+                        client_socket.sendall("ERROR".encode())
+        except Exception as e:
+            logging.error(f"Error with client {address}: {e}")
+            break
+    client_socket.close()
+    logging.info(f"Transaction log for {address}: {transaction_log}")
+def start_server(port):
+    server_socket = socket.socket(socket.AF_INET, socket.SOCK_STREAM)
+    server_socket.bind(('localhost', port))
+    server_socket.listen(2)  # Expecting exactly 2 clients
+    logging.info("Initial Tickets:")
+    for ticket, details in tickets.items():
+        logging.info(f"Ticket #{ticket}, Price: ${details['price']}, Sold: {details['sold']}")
+    clients = []
+    try:
+        while len(clients) &lt; 2:
+            client_socket, addr = server_socket.accept()
+            logging.info(f"Connected with {addr}")
+            client_thread = threading.Thread(target=handle_client, args=(client_socket, addr))
+            client_thread.start()
+            clients.append(client_thread)
+    except KeyboardInterrupt:
+        logging.info("Server is shutting down...")
+    # Wait for all threads to complete
+    for thread in clients:
+        thread.join()
+    logging.info("Final Tickets:")
+    for ticket, details in tickets.items():
+        logging.info(f"Ticket #{ticket}, Price: ${details['price']}, Sold: {details['sold']}")
+    server_socket.close()
+if __name__ == "__main__":
+    random.seed(10)
+    start_server(12345)
+Key Changes:
+Connection Barrier: A threading barrier is used to pause all client threads until exactly two clients have connected. This ensures that the server doesn't begin processing any client requests until both clients are fully connected and ready to transact.
+Error Handling for Barrier: Added handling for potential BrokenBarrierError, which might occur if one of the clients disconnects unexpectedly while waiting at the barrier.
+This modification will fix the issue of premature request processing, aligning with the requirement that the server should handle client requests only after both clients have connected.</t>
+  </si>
+  <si>
+    <t>0/server-0-7.py</t>
+  </si>
+  <si>
+    <t>server-0-7-client-0-6.log</t>
+  </si>
+  <si>
+    <t>client-0-6-1-server-0-7.log, client-0-6-2-server-0-7.log</t>
+  </si>
+  <si>
+    <t>1. Server did not wait for the second client to connect, but proceeded to selling tickets to the first client. 
+2. Client 1 finished first and exited, server exited, and Client 2 was still idling indefinitely
+3. In a message containing the ticket ID and price, the server sent: "1000 3411000 341", causing an error of too many values to unpack.
+4. Error in UDP connection: client-0-6.py", line 29, in udp_listener    udp_sock.bind((hostname, udp_port)) OSError: [WinError 10048] Only one usage of each socket address (protocol/network address/port) is normally permitted</t>
+  </si>
+  <si>
+    <t>1. Fixed
+2. Client 1 finished first and exited, server exited, and Client 2 was still idling indefinitely.
+3. In a message containing the ticket ID and price, the server sent: "1000 3411000 341", causing an error of too many values to unpack. --&gt; DId not happen
+4. Error in UDP connection: client-0-6.py", line 29, in udp_listener    udp_sock.bind((hostname, udp_port)) OSError: [WinError 10048] Only one usage of each socket address (protocol/network address/port) is normally permitted</t>
+  </si>
+  <si>
+    <t>Attached are the server program and the client program that you implemented. However, there are still errors. After completing the transactions, the first client exited, and the server did not wait for the second client to exit, but proceeded to close down the connection, leaving the second client idling indefinitely. The server is supposed to wait for both clients to exit, then log the final ticket database, and close down the connection and exit only when the other client exits. Please fix this problem given the server program and the client program that you implemented.
+Please be sure to log all messages that were sent or received by both server and client. Also, the log mode should be DEBUG to record all levels of information during execution.</t>
+  </si>
+  <si>
+    <t>To address the issue where the server does not properly wait for both clients to exit before shutting down, I will modify the server code to include proper synchronization and client management. Additionally, I'll ensure all communications and events are logged at the DEBUG level, providing detailed visibility into the server's operations.
+Here is a revised approach for the server code:
+Use Thread Joining: Ensure all client handling threads are joined properly before the server attempts to shut down. This guarantees that the server waits for all client transactions to complete.
+Implement Client Tracking: Maintain a list or counter to track active client connections. Only proceed to shutdown when all clients have disconnected.
+Enhanced Logging: Set the logging level to DEBUG and log all incoming and outgoing messages, as well as significant events like client connections, disconnections, and errors.
+Revised Server Code:
+import socket
+import threading
+import random
+import logging
+# Set up logging
+logging.basicConfig(level=logging.DEBUG,  # Set logging to debug level
+                    format='%(asctime)s - %(levelname)s - %(message)s',
+                    handlers=[
+                        logging.FileHandler("ticket_server.log"),
+                        logging.StreamHandler()
+                    ])
+# Lock for thread safety in modifying shared resources
+lock = threading.Lock()
+# Initialize ticket database
+tickets = {f"{10000 + i}": {"price": random.randint(200, 400), "sold": False} for i in range(25)}
+# List to track client threads
+client_threads = []
+def handle_client(client_socket, address):
+    global tickets
+    logging.debug(f"Client connected: {address}")
+    try:
+        while True:
+            data = client_socket.recv(1024).decode('utf-8').strip()
+            if not data:
+                break
+            logging.debug(f"Received from {address}: {data}")
+            cmd, *args = data.split()
+            response = "UNKNOWN COMMAND"
+            with lock:
+                if cmd == "BUY":
+                    user_balance = int(args[0])
+                    for ticket, details in tickets.items():
+                        if not details['sold'] and user_balance &gt;= details['price']:
+                            details['sold'] = True
+                            response = f"{ticket} {details['price']}"
+                            break
+                    else:
+                        response = "SOLDOUT" if all(t['sold'] for t in tickets.values()) else "NOFUNDS"
+                elif cmd == "SELL":
+                    ticket_number = args[0]
+                    if tickets.get(ticket_number, {}).get('sold', False):
+                        tickets[ticket_number]['sold'] = False
+                        response = f"{ticket_number} {tickets[ticket_number]['price']}"
+            client_socket.sendall(response.encode())
+            logging.debug(f"Sent to {address}: {response}")
+    except Exception as e:
+        logging.error(f"Error handling client {address}: {e}")
+    finally:
+        client_socket.close()
+        logging.debug(f"Client disconnected: {address}")
+def start_server(port):
+    server_socket = socket.socket(socket.AF_INET, socket.SOCK_STREAM)
+    server_socket.bind(('localhost', port))
+    server_socket.listen(2)  # Expecting only 2 clients
+    logging.info("Server started and waiting for clients.")
+    try:
+        while len(client_threads) &lt; 2:
+            client_socket, addr = server_socket.accept()
+            thread = threading.Thread(target=handle_client, args=(client_socket, addr))
+            thread.start()
+            client_threads.append(thread)
+        # Wait for all client threads to finish
+        for thread in client_threads:
+            thread.join()
+    finally:
+        logging.info("All clients have disconnected. Final ticket status:")
+        for ticket, details in tickets.items():
+            logging.info(f"Ticket #{ticket}: Price ${details['price']}, Sold {details['sold']}")
+        server_socket.close()
+        logging.info("Server shutdown.")
+if __name__ == "__main__":
+    start_server(12345)
+Key Changes:
+Thread Joining: After starting each client thread, we ensure that the server joins all threads, waiting for each to complete before shutting down.
+Logging: Set to DEBUG level to capture detailed information, ensuring that every message and key action is logged for troubleshooting and analysis.
+This code will ensure that the server properly manages client sessions, waits for all client activities to conclude before shutting down, and provides detailed logging of all interactions and internal states.</t>
+  </si>
+  <si>
+    <t>0/server-0-8.py</t>
+  </si>
+  <si>
+    <t>server-0-8-client-0-6.log</t>
+  </si>
+  <si>
+    <t>client-0-6-1-server-0-8.log, client-0-6-2-server-0-8.log</t>
+  </si>
+  <si>
+    <t>1. Not fixed: Server did not wait for both clients to connect before selling ticket.
+2. Not fixed: Client 1 finished first and exited, server exited, and Client 2 was still idling indefinitely.
+3. In a message containing the ticket ID and price, the server sent: "1000 3411000 341", causing an error of too many values to unpack. --&gt; DId not happen
+4. Error in UDP connection: client-0-6.py", line 29, in udp_listener    udp_sock.bind((hostname, udp_port)) OSError: [WinError 10048] Only one usage of each socket address (protocol/network address/port) is normally permitted
+5. The server program lost some of the original requirements that were already implemented in previous version. Ex: The server did not print the initial database when starting out. The server did not wait for both clients to exit before closing down connections (fixed in exp 0-7).</t>
+  </si>
+  <si>
+    <t>The revised server program that you just generated performed worse than before. The server is supposed to wait for both clients to enter before beginning to sell tickets. Also, the server is supposed to wait for both clients to exit before closing down the connections and exiting the program. Attached is the server program that you generated before last, in which, the server was waiting for both clients to join before processing their buy requests. Based on this server program,  address the second issue, which is waiting for both clients to exit before closing down the connections and exiting the program. 
+Please be sure to log all messages that were sent and received by both of the server and clients. Also, the log mode should be DEBUG to record all levels of information during execution. (Attached the prog. server-0-7.py)</t>
+  </si>
+  <si>
+    <t>To modify the existing server program so that it properly waits for both clients to finish their transactions before shutting down, we'll make sure to handle the joining of client threads effectively. Additionally, I'll ensure that the logging captures all messages and is set to DEBUG level for comprehensive information.
+Here’s a modification based on your requirements:
+Connection and Disconnection Management: Use a barrier to ensure all clients are connected before processing begins. Then, use proper synchronization to ensure all client threads have finished before the server closes any connections and exits.
+Logging: All communications and server operations will be logged at the DEBUG level to provide detailed insights.
+Updated Server Code with Proper Thread Management and Logging
+import socket
+import threading
+import random
+import logging
+# Configure logging
+logging.basicConfig(level=logging.DEBUG,  # Change to DEBUG
+                    format='%(asctime)s - %(levelname)s - %(message)s',
+                    handlers=[
+                        logging.FileHandler("ticket_server.log"),
+                        logging.StreamHandler()
+                    ])
+# Global lock for thread safety
+lock = threading.Lock()
+# Initialize ticket database
+tickets = {f"{10000 + i}": {"price": random.randint(200, 400), "sold": False} for i in range(25)}
+# Connection barrier to ensure both clients are connected before processing starts
+connection_barrier = threading.Barrier(2)  # Waiting for 2 clients
+def handle_client(client_socket, address):
+    global tickets
+    # Wait for both clients to connect
+    connection_barrier.wait()
+    try:
+        while True:
+            data = client_socket.recv(1024)
+            if not data:
+                break
+            data = data.decode('utf-8').strip()
+            logging.debug(f"Received from {address}: {data}")
+            cmd, *args = data.split()
+            with lock:
+                if cmd == "BUY":
+                    user_balance = int(args[0])
+                    response = "SOLDOUT"
+                    for ticket, details in tickets.items():
+                        if not details['sold'] and user_balance &gt;= details['price']:
+                            details['sold'] = True
+                            response = f"{ticket} {details['price']}"
+                            break
+                    client_socket.sendall(response.encode())
+                    logging.debug(f"Sent to {address}: {response}")
+                elif cmd == "SELL":
+                    ticket_number = args[0]
+                    if tickets[ticket_number]['sold']:
+                        tickets[ticket_number]['sold'] = False
+                        response = f"{ticket_number} {tickets[ticket_number]['price']}"
+                        client_socket.sendall(response.encode())
+                        logging.debug(f"Sent to {address}: {response}")
+    except Exception as e:
+        logging.error(f"Error with client {address}: {e}")
+    finally:
+        logging.info(f"Client {address} disconnected.")
+        client_socket.close()
+def start_server(port):
+    server_socket = socket.socket(socket.AF_INET, socket.SOCK_STREAM)
+    server_socket.bind(('localhost', port))
+    server_socket.listen(2)  # Expecting only 2 clients
+    logging.info("Server is ready and waiting for clients.")
+    threads = []
+    try:
+        for _ in range(2):  # We expect exactly 2 clients
+            client_socket, addr = server_socket.accept()
+            logging.info(f"Client {addr} connected.")
+            thread = threading.Thread(target=handle_client, args=(client_socket, addr))
+            thread.start()
+            threads.append(thread)
+        # Wait for all threads to complete
+        for thread in threads:
+            thread.join()
+    finally:
+        logging.info("All clients have disconnected. Final ticket database:")
+        for ticket, details in tickets.items():
+            logging.info(f"Ticket #{ticket}: Price ${details['price']}, Sold {details['sold']}")
+        server_socket.close()
+        logging.info("Server has shut down.")
+if __name__ == "__main__":
+    start_server(12345)
+Explanation
+Connection Synchronization: A barrier ensures all clients are connected before any transactions start.
+Thread Joining: After starting client threads, the server waits for all to complete before proceeding to shut down. This ensures that the server only shuts down after all clients have disconnected.
+Logging: All incoming and outgoing messages are logged at the DEBUG level to provide a detailed execution trace.
+This approach should resolve the issues with client handling and shutdown synchronization, ensuring that the server behaves as expected throughout its lifecycle.</t>
+  </si>
+  <si>
+    <t>0/server-0-9.py</t>
+  </si>
+  <si>
+    <t>server-0-9-client-0-6.log</t>
+  </si>
+  <si>
+    <t>client-0-6-1-server-0-9.log, client-0-6-2-server-0-9.log</t>
+  </si>
+  <si>
+    <t>This implementation did not cover all the functionalities of the server. What happen when the server receives a buy request that is insufficient from a client?
+You also forgot to print out the initial ticket database when the server just started, which is one of the required functionalities of the server.</t>
+  </si>
+  <si>
+    <t>To ensure that the server prints the initial ticket database when it starts, I'll include a function that logs the initial state of the ticket database right after it is initialized. This will give you visibility into the ticket setup before any transactions occur.
+Here’s the modified server code to include this functionality:
+import socket
+import threading
+import random
+import logging
+# Configure logging
+logging.basicConfig(level=logging.DEBUG,
+                    format='%(asctime)s - %(levelname)s - %(message)s',
+                    handlers=[
+                        logging.FileHandler("ticket_server.log"),
+                        logging.StreamHandler()
+                    ])
+# Global lock for thread safety
+lock = threading.Lock()
+# Initialize ticket database
+tickets = {f"{10000 + i}": {"price": random.randint(200, 400), "sold": False} for i in range(25)}
+# Connection barrier to ensure both clients are connected before processing starts
+connection_barrier = threading.Barrier(2)  # Waiting for 2 clients
+def print_initial_tickets():
+    """Prints the initial state of the tickets."""
+    logging.info("Initial ticket database:")
+    for ticket, details in tickets.items():
+        logging.info(f"Ticket #{ticket}: Price ${details['price']}, Sold {details['sold']}")
+def handle_client(client_socket, address):
+    global tickets
+    # Wait for both clients to connect
+    connection_barrier.wait()
+    try:
+        while True:
+            data = client_socket.recv(1024)
+            if not data:
+                break
+            data = data.decode('utf-8').strip()
+            logging.debug(f"Received from {address}: {data}")
+            cmd, *args = data.split()
+            response = "UNKNOWN COMMAND"
+            if cmd == "BUY":
+                user_balance = int(args[0])
+                with lock:
+                    for ticket, details in tickets.items():
+                        if not details['sold']:
+                            if user_balance &gt;= details['price']:
+                                details['sold'] = True
+                                response = f"{ticket} {details['price']}"
+                                break
+                            else:
+                                response = "NOFUNDS"
+                        else:
+                            response = "SOLDOUT"
+                client_socket.sendall(response.encode())
+                logging.debug(f"Sent to {address}: {response}")
+            elif cmd == "SELL":
+                ticket_number = args[0]
+                with lock:
+                    if tickets[ticket_number]['sold']:
+                        tickets[ticket_number]['sold'] = False
+                        response = f"{ticket_number} {tickets[ticket_number]['price']}"
+                        client_socket.sendall(response.encode())
+                        logging.debug(f"Sent to {address}: {response}")
+    except Exception as e:
+        logging.error(f"Error with client {address}: {e}")
+    finally:
+        logging.info(f"Client {address} disconnected.")
+        client_socket.close()
+def start_server(port):
+    server_socket = socket.socket(socket.AF_INET, socket.SOCK_STREAM)
+    server_socket.bind(('localhost', port))
+    server_socket.listen(2)  # Expecting only 2 clients
+    logging.info("Server is ready and waiting for clients.")
+    print_initial_tickets()  # Log the initial state of the ticket database
+    threads = []
+    try:
+        for _ in range(2):  # We expect exactly 2 clients
+            client_socket, addr = server_socket.accept()
+            logging.info(f"Client {addr} connected.")
+            thread = threading.Thread(target=handle_client, args=(client_socket, addr))
+            thread.start()
+            threads.append(thread)
+        # Wait for all threads to complete
+        for thread in threads:
+            thread.join()
+    finally:
+        logging.info("All clients have disconnected. Final ticket database:")
+        for ticket, details in tickets.items():
+            logging.info(f"Ticket #{ticket}: Price ${details['price']}, Sold {details['sold']}")
+        server_socket.close()
+        logging.info("Server has shut down.")
+if __name__ == "__main__":
+    start_server(12345)
+Key Adjustments:
+Handling Insufficient Funds: The server checks if the client's balance is enough for the cheapest available ticket. If not, it responds with "NOFUNDS".
+Print Initial Tickets: The print_initial_tickets() function is called right after the server starts and the tickets are initialized. This ensures the initial state of the ticket database is logged.
+Improved Logging: The initial and final state of tickets are clearly logged, along with all client transactions and connections, ensuring full traceability.
+This code now meets all specified requirements, including waiting for both clients to connect before transactions begin, handling buy requests with insufficient funds appropriately, and logging the initial ticket state.</t>
+  </si>
+  <si>
+    <t>0/server-0-10.py</t>
+  </si>
+  <si>
+    <t>server-0-10-client-0-6.log</t>
+  </si>
+  <si>
+    <t>client-0-6-1-server-0-10.log, client-0-6-2-server-0-10.log</t>
+  </si>
+  <si>
+    <t>1. Fixed given the server-0-7 as input: Server did not wait for both clients to connect before selling ticket.
+2. Client 1 finished first and exited, server exited, and Client 2 was still idling indefinitely. --&gt; The issue is not on the server side. The issue is related to error 4, when one of the last client closed the TCP connection, but still waiting for the UDP thread to finish.
+3. In a message containing the ticket ID and price, the server sent: "1000 3411000 341", causing an error of too many values to unpack. --&gt; DId not happen
+4. Error in UDP connection: client-0-6.py", line 29, in udp_listener    udp_sock.bind((hostname, udp_port)) OSError: [WinError 10048] Only one usage of each socket address (protocol/network address/port) is normally permitted
+5. The server program lost some of the original requirements that were already implemented in previous version. Ex: The server did not print the initial database when starting out. The server did not wait for both clients to exit before closing down connections (fixed in exp 0-7).
+6. Missing a condition to handle NOFUNDS, when the client does not have enough money to buy a ticket.
+7. A client still waits for the UDP listener to finish.</t>
+  </si>
+  <si>
+    <t>1. Fixed given the server-0-7 as input: Server did not wait for both clients to connect before selling ticket.
+2. Client 1 finished first and exited, server exited, and Client 2 was still idling indefinitely. --&gt; The issue is not on the server side. The issue is related to error 4, when one of the last client closed the TCP connection, but still waiting for the UDP thread to finish.
+3. In a message containing the ticket ID and price, the server sent: "1000 3411000 341", causing an error of too many values to unpack. --&gt; DId not happen
+4. Error in UDP connection: client-0-6.py", line 29, in udp_listener    udp_sock.bind((hostname, udp_port)) OSError: [WinError 10048] Only one usage of each socket address (protocol/network address/port) is normally permitted
+5. Fixed: The server program lost some of the original requirements that were already implemented in previous version. Ex: The server did not print the initial database when starting out. The server did not wait for both clients to exit before closing down connections (fixed in exp 0-7).
+6. Missing a condition to handle NOFUNDS, when the client does not have enough money to buy a ticket.
+7. A client still waits for the UDP listener to finish.</t>
   </si>
 </sst>
 </file>
@@ -774,24 +1344,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E39F754-1327-4C31-8156-C5B4C2CFB3FA}">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.140625" customWidth="1"/>
-    <col min="3" max="3" width="12.28515625" customWidth="1"/>
+    <col min="1" max="1" width="4.7109375" customWidth="1"/>
+    <col min="2" max="2" width="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" customWidth="1"/>
     <col min="4" max="4" width="19.140625" customWidth="1"/>
     <col min="5" max="5" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="69.42578125" customWidth="1"/>
+    <col min="6" max="6" width="19.85546875" customWidth="1"/>
+    <col min="7" max="7" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.42578125" customWidth="1"/>
+    <col min="9" max="9" width="69.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -808,13 +1381,19 @@
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -830,11 +1409,11 @@
       <c r="E2" t="s">
         <v>11</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0</v>
       </c>
@@ -850,11 +1429,11 @@
       <c r="E3" t="s">
         <v>11</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>0</v>
       </c>
@@ -871,13 +1450,16 @@
         <v>14</v>
       </c>
       <c r="F4" t="s">
+        <v>29</v>
+      </c>
+      <c r="G4" t="s">
         <v>11</v>
       </c>
-      <c r="G4" t="s">
+      <c r="I4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>0</v>
       </c>
@@ -894,13 +1476,16 @@
         <v>18</v>
       </c>
       <c r="F5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G5" t="s">
         <v>11</v>
       </c>
-      <c r="G5" t="s">
+      <c r="I5" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>0</v>
       </c>
@@ -916,11 +1501,156 @@
       <c r="E6" t="s">
         <v>22</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>11</v>
       </c>
-      <c r="G6" t="s">
+      <c r="I6" t="s">
         <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>0</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F7" t="s">
+        <v>31</v>
+      </c>
+      <c r="G7" t="s">
+        <v>25</v>
+      </c>
+      <c r="H7" t="s">
+        <v>32</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>0</v>
+      </c>
+      <c r="B8">
+        <v>7</v>
+      </c>
+      <c r="C8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E8" t="s">
+        <v>35</v>
+      </c>
+      <c r="F8" t="s">
+        <v>36</v>
+      </c>
+      <c r="G8" t="s">
+        <v>25</v>
+      </c>
+      <c r="H8" t="s">
+        <v>37</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>0</v>
+      </c>
+      <c r="B9">
+        <v>8</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E9" t="s">
+        <v>42</v>
+      </c>
+      <c r="F9" t="s">
+        <v>43</v>
+      </c>
+      <c r="G9" t="s">
+        <v>25</v>
+      </c>
+      <c r="H9" t="s">
+        <v>44</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>0</v>
+      </c>
+      <c r="B10">
+        <v>9</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E10" t="s">
+        <v>48</v>
+      </c>
+      <c r="F10" t="s">
+        <v>49</v>
+      </c>
+      <c r="G10" t="s">
+        <v>25</v>
+      </c>
+      <c r="H10" t="s">
+        <v>50</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>0</v>
+      </c>
+      <c r="B11">
+        <v>10</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E11" t="s">
+        <v>53</v>
+      </c>
+      <c r="F11" t="s">
+        <v>54</v>
+      </c>
+      <c r="G11" t="s">
+        <v>25</v>
+      </c>
+      <c r="H11" t="s">
+        <v>55</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added experiment report 0804
</commit_message>
<xml_diff>
--- a/Experiment Tracking Sheet.xlsx
+++ b/Experiment Tracking Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\natal\Desktop\DIssertation\Ticket5ellingSystem-Exp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98347EA5-A43F-40ED-8E37-183E086E951B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C28CEEE-7F08-4766-9133-A86E1E50FFA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23148" yWindow="5880" windowWidth="23256" windowHeight="12456" xr2:uid="{20830222-D529-4FF8-BDA5-3DAE3BD48417}"/>
   </bookViews>
@@ -974,7 +974,7 @@
 3. In a message containing the ticket ID and price, the server sent: "1000 3411000 341", causing an error of too many values to unpack. --&gt; DId not happen
 4. Error in UDP connection: client-0-6.py", line 29, in udp_listener    udp_sock.bind((hostname, udp_port)) OSError: [WinError 10048] Only one usage of each socket address (protocol/network address/port) is normally permitted
 5. Fixed: The server program lost some of the original requirements that were already implemented in previous version. Ex: The server did not print the initial database when starting out. The server did not wait for both clients to exit before closing down connections (fixed in exp 0-7).
-6. Missing a condition to handle NOFUNDS, when the client does not have enough money to buy a ticket.
+6. Fixed: Missing a condition to handle NOFUNDS, when the client does not have enough money to buy a ticket.
 7. A client still waits for the UDP listener to finish.</t>
   </si>
 </sst>
@@ -1028,8 +1028,8 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1347,8 +1347,8 @@
   <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I11" sqref="I11"/>
+      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1403,7 +1403,7 @@
       <c r="C2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" t="s">
         <v>8</v>
       </c>
       <c r="E2" t="s">
@@ -1420,10 +1420,10 @@
       <c r="B3">
         <v>2</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" t="s">
         <v>10</v>
       </c>
       <c r="E3" t="s">
@@ -1443,7 +1443,7 @@
       <c r="C4" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" t="s">
         <v>13</v>
       </c>
       <c r="E4" t="s">
@@ -1469,7 +1469,7 @@
       <c r="C5" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" t="s">
         <v>17</v>
       </c>
       <c r="E5" t="s">
@@ -1492,10 +1492,10 @@
       <c r="B6">
         <v>5</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" t="s">
         <v>21</v>
       </c>
       <c r="E6" t="s">
@@ -1518,7 +1518,7 @@
       <c r="C7" t="s">
         <v>24</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" t="s">
         <v>26</v>
       </c>
       <c r="E7" t="s">
@@ -1533,7 +1533,7 @@
       <c r="H7" t="s">
         <v>32</v>
       </c>
-      <c r="I7" s="2" t="s">
+      <c r="I7" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1547,7 +1547,7 @@
       <c r="C8" t="s">
         <v>33</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" t="s">
         <v>34</v>
       </c>
       <c r="E8" t="s">
@@ -1562,7 +1562,7 @@
       <c r="H8" t="s">
         <v>37</v>
       </c>
-      <c r="I8" s="2" t="s">
+      <c r="I8" s="3" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1573,10 +1573,10 @@
       <c r="B9">
         <v>8</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" t="s">
         <v>40</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" t="s">
         <v>41</v>
       </c>
       <c r="E9" t="s">
@@ -1591,7 +1591,7 @@
       <c r="H9" t="s">
         <v>44</v>
       </c>
-      <c r="I9" s="2" t="s">
+      <c r="I9" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1602,10 +1602,10 @@
       <c r="B10">
         <v>9</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" t="s">
         <v>46</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D10" t="s">
         <v>47</v>
       </c>
       <c r="E10" t="s">
@@ -1620,7 +1620,7 @@
       <c r="H10" t="s">
         <v>50</v>
       </c>
-      <c r="I10" s="2" t="s">
+      <c r="I10" t="s">
         <v>56</v>
       </c>
     </row>
@@ -1631,10 +1631,10 @@
       <c r="B11">
         <v>10</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" t="s">
         <v>51</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D11" t="s">
         <v>52</v>
       </c>
       <c r="E11" t="s">
@@ -1649,7 +1649,7 @@
       <c r="H11" t="s">
         <v>55</v>
       </c>
-      <c r="I11" s="2" t="s">
+      <c r="I11" s="3" t="s">
         <v>57</v>
       </c>
     </row>

</xml_diff>